<commit_message>
Added Driver License ID to the IEPD.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Firearm_Registration_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Firearm_Registration_Query_Results-mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Firearm_Registration_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Firearm_Registration_Query_Results-mapping.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="465" windowWidth="19290" windowHeight="7305"/>
+    <workbookView xWindow="-27820" yWindow="6320" windowWidth="32380" windowHeight="15440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="195">
   <si>
     <t>Business Class</t>
   </si>
@@ -589,13 +594,25 @@
   </si>
   <si>
     <t>nc:ContactInformationType</t>
+  </si>
+  <si>
+    <t>Driver License</t>
+  </si>
+  <si>
+    <t>nc:IdentificationType</t>
+  </si>
+  <si>
+    <t>Driver License ID</t>
+  </si>
+  <si>
+    <t>exchange:FirearmRegistrationQueryResults/nc:DriverLicense/nc:DriverLicenseIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -618,6 +635,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -636,15 +669,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -944,25 +981,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="41.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1"/>
-    <col min="5" max="5" width="38.42578125" customWidth="1"/>
-    <col min="6" max="6" width="137.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="41.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="42.5" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" customWidth="1"/>
+    <col min="5" max="5" width="38.5" customWidth="1"/>
+    <col min="6" max="6" width="137.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -988,7 +1025,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1002,7 +1039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1025,7 +1062,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="B4" t="s">
         <v>55</v>
       </c>
@@ -1045,7 +1082,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="B5" t="s">
         <v>92</v>
       </c>
@@ -1062,7 +1099,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="B6" t="s">
         <v>93</v>
       </c>
@@ -1082,7 +1119,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="B7" t="s">
         <v>56</v>
       </c>
@@ -1102,7 +1139,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" t="s">
         <v>58</v>
       </c>
@@ -1119,7 +1156,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="B9" t="s">
         <v>59</v>
       </c>
@@ -1139,7 +1176,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="B10" t="s">
         <v>61</v>
       </c>
@@ -1159,7 +1196,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="B11" t="s">
         <v>63</v>
       </c>
@@ -1179,7 +1216,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="B12" t="s">
         <v>64</v>
       </c>
@@ -1196,7 +1233,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="B13" t="s">
         <v>21</v>
       </c>
@@ -1213,7 +1250,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="B14" t="s">
         <v>65</v>
       </c>
@@ -1233,7 +1270,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="B15" t="s">
         <v>67</v>
       </c>
@@ -1253,7 +1290,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="B16" t="s">
         <v>69</v>
       </c>
@@ -1270,7 +1307,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="B17" t="s">
         <v>70</v>
       </c>
@@ -1287,7 +1324,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="B18" t="s">
         <v>71</v>
       </c>
@@ -1307,7 +1344,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="B19" t="s">
         <v>72</v>
       </c>
@@ -1324,7 +1361,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1344,7 +1381,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="B22" t="s">
         <v>22</v>
       </c>
@@ -1361,7 +1398,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="B23" t="s">
         <v>23</v>
       </c>
@@ -1378,7 +1415,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="B24" t="s">
         <v>24</v>
       </c>
@@ -1398,7 +1435,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="B25" t="s">
         <v>25</v>
       </c>
@@ -1415,7 +1452,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="B26" t="s">
         <v>125</v>
       </c>
@@ -1435,7 +1472,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="B27" t="s">
         <v>126</v>
       </c>
@@ -1452,7 +1489,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="B28" t="s">
         <v>127</v>
       </c>
@@ -1469,7 +1506,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="B29" t="s">
         <v>128</v>
       </c>
@@ -1486,7 +1523,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="B30" t="s">
         <v>129</v>
       </c>
@@ -1503,7 +1540,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -1523,7 +1560,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="B33" t="s">
         <v>13</v>
       </c>
@@ -1543,7 +1580,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="B34" t="s">
         <v>38</v>
       </c>
@@ -1563,7 +1600,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="B35" t="s">
         <v>41</v>
       </c>
@@ -1580,7 +1617,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="B36" t="s">
         <v>140</v>
       </c>
@@ -1597,7 +1634,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="B37" t="s">
         <v>141</v>
       </c>
@@ -1611,7 +1648,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="B38" t="s">
         <v>142</v>
       </c>
@@ -1631,7 +1668,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="B39" t="s">
         <v>4</v>
       </c>
@@ -1648,311 +1685,336 @@
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
+        <v>191</v>
+      </c>
+      <c r="B41" t="s">
+        <v>193</v>
+      </c>
+      <c r="C41" t="s">
+        <v>192</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
         <v>148</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>188</v>
-      </c>
-      <c r="C41" t="s">
-        <v>153</v>
-      </c>
-      <c r="D41" t="s">
-        <v>151</v>
-      </c>
-      <c r="E41" t="s">
-        <v>33</v>
-      </c>
-      <c r="F41" t="s">
-        <v>155</v>
-      </c>
-      <c r="H41" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>145</v>
-      </c>
-      <c r="C42" t="s">
-        <v>153</v>
-      </c>
-      <c r="D42" t="s">
-        <v>94</v>
-      </c>
-      <c r="E42" t="s">
-        <v>16</v>
-      </c>
-      <c r="F42" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>146</v>
       </c>
       <c r="C43" t="s">
         <v>153</v>
       </c>
       <c r="D43" t="s">
-        <v>95</v>
+        <v>151</v>
       </c>
       <c r="E43" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="F43" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H43" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="B44" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C44" t="s">
         <v>153</v>
       </c>
       <c r="D44" t="s">
+        <v>94</v>
+      </c>
+      <c r="E44" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="B45" t="s">
+        <v>146</v>
+      </c>
+      <c r="C45" t="s">
+        <v>153</v>
+      </c>
+      <c r="D45" t="s">
+        <v>95</v>
+      </c>
+      <c r="E45" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" t="s">
+        <v>157</v>
+      </c>
+      <c r="H45" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="B46" t="s">
+        <v>147</v>
+      </c>
+      <c r="C46" t="s">
+        <v>153</v>
+      </c>
+      <c r="D46" t="s">
         <v>154</v>
-      </c>
-      <c r="E44" t="s">
-        <v>15</v>
-      </c>
-      <c r="F44" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>149</v>
-      </c>
-      <c r="B46" t="s">
-        <v>150</v>
-      </c>
-      <c r="C46" t="s">
-        <v>190</v>
-      </c>
-      <c r="D46" t="s">
-        <v>159</v>
       </c>
       <c r="E46" t="s">
         <v>15</v>
       </c>
       <c r="F46" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>149</v>
+      </c>
+      <c r="B48" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" t="s">
+        <v>190</v>
+      </c>
+      <c r="D48" t="s">
+        <v>159</v>
+      </c>
+      <c r="E48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="50" spans="1:8">
+      <c r="A50" t="s">
         <v>36</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B50" t="s">
         <v>163</v>
-      </c>
-      <c r="C48" t="s">
-        <v>161</v>
-      </c>
-      <c r="D48" t="s">
-        <v>45</v>
-      </c>
-      <c r="E48" t="s">
-        <v>46</v>
-      </c>
-      <c r="F48" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>164</v>
-      </c>
-      <c r="C49" t="s">
-        <v>161</v>
-      </c>
-      <c r="D49" t="s">
-        <v>47</v>
-      </c>
-      <c r="E49" t="s">
-        <v>46</v>
-      </c>
-      <c r="F49" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>165</v>
       </c>
       <c r="C50" t="s">
         <v>161</v>
       </c>
       <c r="D50" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E50" t="s">
         <v>46</v>
       </c>
       <c r="F50" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>162</v>
-      </c>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="B51" t="s">
+        <v>164</v>
+      </c>
+      <c r="C51" t="s">
+        <v>161</v>
+      </c>
+      <c r="D51" t="s">
+        <v>47</v>
+      </c>
+      <c r="E51" t="s">
+        <v>46</v>
+      </c>
+      <c r="F51" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="B52" t="s">
         <v>165</v>
       </c>
       <c r="C52" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D52" t="s">
-        <v>168</v>
+        <v>48</v>
       </c>
       <c r="E52" t="s">
         <v>46</v>
       </c>
       <c r="F52" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
+        <v>162</v>
+      </c>
+      <c r="B54" t="s">
+        <v>165</v>
+      </c>
+      <c r="C54" t="s">
+        <v>167</v>
+      </c>
+      <c r="D54" t="s">
+        <v>168</v>
+      </c>
+      <c r="E54" t="s">
+        <v>46</v>
+      </c>
+      <c r="F54" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+    <row r="55" spans="1:8">
+      <c r="B55" t="s">
         <v>166</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C55" t="s">
         <v>167</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D55" t="s">
         <v>169</v>
-      </c>
-      <c r="E53" t="s">
-        <v>46</v>
-      </c>
-      <c r="F53" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>172</v>
-      </c>
-      <c r="B55" t="s">
-        <v>165</v>
-      </c>
-      <c r="C55" t="s">
-        <v>174</v>
-      </c>
-      <c r="D55" t="s">
-        <v>168</v>
       </c>
       <c r="E55" t="s">
         <v>46</v>
       </c>
       <c r="F55" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
+        <v>172</v>
+      </c>
+      <c r="B57" t="s">
+        <v>165</v>
+      </c>
+      <c r="C57" t="s">
+        <v>174</v>
+      </c>
+      <c r="D57" t="s">
+        <v>168</v>
+      </c>
+      <c r="E57" t="s">
+        <v>46</v>
+      </c>
+      <c r="F57" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+    <row r="58" spans="1:8">
+      <c r="B58" t="s">
         <v>173</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C58" t="s">
         <v>174</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D58" t="s">
         <v>175</v>
-      </c>
-      <c r="E56" t="s">
-        <v>46</v>
-      </c>
-      <c r="F56" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>178</v>
-      </c>
-      <c r="B58" t="s">
-        <v>165</v>
-      </c>
-      <c r="C58" t="s">
-        <v>179</v>
-      </c>
-      <c r="D58" t="s">
-        <v>180</v>
       </c>
       <c r="E58" t="s">
         <v>46</v>
       </c>
       <c r="F58" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" t="s">
+        <v>178</v>
+      </c>
+      <c r="B60" t="s">
+        <v>165</v>
+      </c>
+      <c r="C60" t="s">
+        <v>179</v>
+      </c>
+      <c r="D60" t="s">
+        <v>180</v>
+      </c>
+      <c r="E60" t="s">
+        <v>46</v>
+      </c>
+      <c r="F60" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+    <row r="61" spans="1:8">
+      <c r="B61" t="s">
         <v>189</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C61" t="s">
         <v>179</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D61" t="s">
         <v>181</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E61" t="s">
         <v>33</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F61" t="s">
         <v>184</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H61" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="63" spans="1:8">
+      <c r="A63" t="s">
         <v>185</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B63" t="s">
         <v>37</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C63" t="s">
         <v>174</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D63" t="s">
         <v>168</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E63" t="s">
         <v>46</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F63" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+    <row r="64" spans="1:8">
+      <c r="B64" t="s">
         <v>173</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C64" t="s">
         <v>174</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D64" t="s">
         <v>175</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E64" t="s">
         <v>46</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F64" t="s">
         <v>186</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1962,9 +2024,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1974,8 +2041,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>